<commit_message>
Completed Question 7 on 5
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nss_data_analytics\Projects\lookups-budget-JEmmonsJR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2CCE3A-FD7C-4A65-8DE2-90B424290721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5875A3C8-5E31-4CC0-A1DA-0738C8AA95DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -879,6 +879,978 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>metro_budget!$B$82</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Community Education Commission</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>443300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>495200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>487500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0AA7-49C2-80DB-A8A6BD330F45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>407090.37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>467907.84000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>478318.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0AA7-49C2-80DB-A8A6BD330F45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1936060208"/>
+        <c:axId val="1802435936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1936060208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1802435936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1802435936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1936060208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A0D5043-2F27-1F78-7578-D88661AE2030}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1178,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4524,15 +5496,15 @@
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX($D$2:$D$52,MATCH($A74,$A$2:$A$52))</f>
+        <f>INDEX($A$2:$P$52,MATCH($A74,$A$2:$A$52),MATCH(B$73,$A$1:$P$1))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f>INDEX($I$2:$I$52,MATCH($A74,$A$2:$A$52))</f>
+        <f t="shared" ref="C74:D79" si="15">INDEX($A$2:$P$52,MATCH($A74,$A$2:$A$52),MATCH(C$73,$A$1:$P$1))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f>INDEX($N$2:$N$52,MATCH($A74,$A$2:$A$52))</f>
+        <f t="shared" si="15"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4541,15 +5513,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="15">INDEX($D$2:$D$52,MATCH($A75,$A$2:$A$52))</f>
+        <f t="shared" ref="B75:B79" si="16">INDEX($A$2:$P$52,MATCH($A75,$A$2:$A$52),MATCH(B$73,$A$1:$P$1))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="16">INDEX($I$2:$I$52,MATCH($A75,$A$2:$A$52))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="17">INDEX($N$2:$N$52,MATCH($A75,$A$2:$A$52))</f>
+        <f t="shared" si="15"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4558,15 +5530,15 @@
         <v>32</v>
       </c>
       <c r="B76">
+        <f t="shared" si="16"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
         <f t="shared" si="15"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C76">
-        <f t="shared" si="16"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4575,15 +5547,15 @@
         <v>38</v>
       </c>
       <c r="B77">
+        <f t="shared" si="16"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
         <f t="shared" si="15"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C77">
-        <f t="shared" si="16"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4592,15 +5564,15 @@
         <v>39</v>
       </c>
       <c r="B78">
+        <f t="shared" si="16"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
         <f t="shared" si="15"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C78">
-        <f t="shared" si="16"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4609,15 +5581,15 @@
         <v>55</v>
       </c>
       <c r="B79">
+        <f t="shared" si="16"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
         <f t="shared" si="15"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C79">
-        <f t="shared" si="16"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4631,7 +5603,7 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4648,26 +5620,38 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B$2:B$52,MATCH($B$82,$A$2:$A$52))</f>
-        <v>356640100</v>
+        <v>443300</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C$2:C$52,MATCH($B$82,$A$2:$A$52))</f>
-        <v>341243679.13</v>
+        <v>407090.37</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
+      <c r="B85" s="6">
+        <f>INDEX(G$2:G$52,MATCH($B$82,$A$2:$A$52))</f>
+        <v>495200</v>
+      </c>
+      <c r="C85" s="6">
+        <f>INDEX(H$2:H$52,MATCH($B$82,$A$2:$A$52))</f>
+        <v>467907.84000000003</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
+      <c r="B86" s="6">
+        <f>INDEX(L$2:L$52,MATCH($B$82,$A$2:$A$52))</f>
+        <v>487500</v>
+      </c>
+      <c r="C86" s="6">
+        <f>INDEX(M$2:M$52,MATCH($B$82,$A$2:$A$52))</f>
+        <v>478318.92</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
@@ -4813,6 +5797,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Completed Question 8 no bonus
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nss_data_analytics\Projects\lookups-budget-JEmmonsJR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6F88C-6B6C-4F37-8411-1528E62FBFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E16978-2563-422B-BE14-9DC9F8F5CB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2150,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5698,25 +5698,88 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP(B$89,$F$2:$F$52,$A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91" s="5">
+        <f>_xlfn.XLOOKUP(B91,$A$2:$A$52,$E$2:$E$52)</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP(D$89,$F$2:$F$52,$A$2:$A$52)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E91" s="5">
+        <f>_xlfn.XLOOKUP(D91,$A$2:$A$52,$E$2:$E$52)</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP(F$89,$F$2:$F$52,$A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G91" s="5">
+        <f>_xlfn.XLOOKUP(F91,$A$2:$A$52,$E$2:$E$52)</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP(B$89,$K$2:$K$52,$A$2:$A$52)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C92" s="5">
+        <f>_xlfn.XLOOKUP(B92,$A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP(D$89,$K$2:$K$52,$A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E92" s="5">
+        <f>_xlfn.XLOOKUP(D92,$A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F92" t="str">
+        <f>_xlfn.XLOOKUP(F$89,$K$2:$K$52,$A$2:$A$52)</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G92" s="5">
+        <f>_xlfn.XLOOKUP(F92,$A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.13918241656366656</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP(B$89,$P$2:$P$52,$A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C93" s="5">
+        <f>_xlfn.XLOOKUP(B93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D93" t="str">
+        <f>_xlfn.XLOOKUP(D$89,$P$2:$P$52,$A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E93" s="5">
+        <f>_xlfn.XLOOKUP(D93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F93" t="str">
+        <f>_xlfn.XLOOKUP(F$89,$P$2:$P$52,$A$2:$A$52)</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G93" s="5">
+        <f>_xlfn.XLOOKUP(F93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.12882667147667154</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">

</xml_diff>